<commit_message>
Small changes for visual presentation
</commit_message>
<xml_diff>
--- a/SRC/DetailedCropsData.xlsx
+++ b/SRC/DetailedCropsData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Farm Name</t>
   </si>
@@ -62,7 +62,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>Hello</t>
+    <t>Strawberries</t>
   </si>
   <si>
     <t>555</t>
@@ -71,24 +71,18 @@
     <t>10/10/2022</t>
   </si>
   <si>
-    <t>Rivera Farms</t>
-  </si>
-  <si>
-    <t>Tulare</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Apples</t>
-  </si>
-  <si>
-    <t>2024-01-01</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
+    <t>Mandarines</t>
+  </si>
+  <si>
+    <t>05-01-2024</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Grapes</t>
   </si>
   <si>
@@ -96,6 +90,42 @@
   </si>
   <si>
     <t>10-10-2023</t>
+  </si>
+  <si>
+    <t>Pomona Farms</t>
+  </si>
+  <si>
+    <t>Pomona, CA</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Blueberries</t>
+  </si>
+  <si>
+    <t>987</t>
+  </si>
+  <si>
+    <t>2024-03-29</t>
+  </si>
+  <si>
+    <t>CPP Farms</t>
+  </si>
+  <si>
+    <t>Cal Poly Vista</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Pears</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2023-08-03</t>
   </si>
 </sst>
 </file>
@@ -140,7 +170,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -217,25 +247,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="D4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="E4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="G4" t="s" s="0">
         <v>22</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -246,19 +276,65 @@
         <v>13</v>
       </c>
       <c r="C5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="F5" t="s" s="0">
         <v>25</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>27</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>